<commit_message>
My all work was failed
</commit_message>
<xml_diff>
--- a/files/res.xlsx
+++ b/files/res.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenServer\domains\excel.loc\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62FA0252-7032-4E7F-B581-8D057A9211FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBCEC0B5-4A7E-45D8-9AF1-3EE98C10174E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="599" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="599" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidelines" sheetId="8" r:id="rId1"/>
     <sheet name="Sample Calculator" sheetId="1" r:id="rId2"/>
-    <sheet name="Validation" sheetId="7" state="hidden" r:id="rId3"/>
-    <sheet name="Tax Calculations" sheetId="5" state="hidden" r:id="rId4"/>
-    <sheet name="HEM Table" sheetId="6" state="hidden" r:id="rId5"/>
+    <sheet name="Validation" sheetId="7" r:id="rId3"/>
+    <sheet name="Tax Calculations" sheetId="5" r:id="rId4"/>
+    <sheet name="HEM Table" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Applicant1IndividialCoupleWith">Validation!$B$42</definedName>
@@ -35,7 +35,7 @@
     <definedName name="Validstatus3">Validation!$G$2:$G$5</definedName>
     <definedName name="Validstatus4">Validation!$G$2:$G$5</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2168,12 +2168,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Comma 2" xfId="4" xr:uid="{BBCE6B80-E6CA-4473-A4DF-3744C6B2EBB3}"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
     <cellStyle name="Currency 2" xfId="5" xr:uid="{F518726C-C1F0-4E27-8C7D-A833CC62DCD5}"/>
-    <cellStyle name="Денежный" xfId="3" builtinId="4"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Процентный" xfId="2" builtinId="5"/>
-    <cellStyle name="Финансовый" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="27">
     <dxf>
@@ -2708,9 +2708,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2748,7 +2748,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2854,7 +2854,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3243,8 +3243,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:DR152"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE21" sqref="AE21"/>
+    <sheetView showGridLines="0" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93:I93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18153,7 +18153,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:P116"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>

</xml_diff>